<commit_message>
Added upload & display assets & more docs
</commit_message>
<xml_diff>
--- a/GetAgent Docs/SRS.xlsx
+++ b/GetAgent Docs/SRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\Self Projects\GetAgent\GetAgent Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6946337-D1DF-4EE3-A25F-0F2DAD54852B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD66EDDE-F2A4-4EBF-9994-A54531F144DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2376" windowWidth="17280" windowHeight="7296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -243,9 +243,6 @@
     <t xml:space="preserve">מפרסם באתר פרטיי נכס חדש למכירה/השכרה </t>
   </si>
   <si>
-    <t>התנקות</t>
-  </si>
-  <si>
     <t>מתנתק מהחשבון</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>שולח פרטיי לקוח</t>
+  </si>
+  <si>
+    <t>התנתקות</t>
   </si>
 </sst>
 </file>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="K25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1162,16 +1162,16 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G24" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -1233,13 +1233,13 @@
         <v>47</v>
       </c>
       <c r="L32" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M32" s="28" t="s">
         <v>61</v>
       </c>
       <c r="N32" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.25">
@@ -1247,13 +1247,13 @@
         <v>48</v>
       </c>
       <c r="L33" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M33" s="28" t="s">
         <v>61</v>
       </c>
       <c r="N33" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.25">
@@ -1317,13 +1317,13 @@
         <v>53</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M38" s="28" t="s">
         <v>60</v>
       </c>
       <c r="N38" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="11:14" x14ac:dyDescent="0.25">
@@ -1331,13 +1331,13 @@
         <v>54</v>
       </c>
       <c r="L39" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M39" s="28" t="s">
         <v>60</v>
       </c>
       <c r="N39" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.25">
@@ -1345,13 +1345,13 @@
         <v>55</v>
       </c>
       <c r="L40" s="28" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="M40" s="28" t="s">
         <v>61</v>
       </c>
       <c r="N40" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.25">
@@ -1359,13 +1359,13 @@
         <v>56</v>
       </c>
       <c r="L41" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M41" s="28" t="s">
         <v>16</v>
       </c>
       <c r="N41" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="11:14" x14ac:dyDescent="0.25">
@@ -1373,13 +1373,13 @@
         <v>57</v>
       </c>
       <c r="L42" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M42" s="28" t="s">
         <v>16</v>
       </c>
       <c r="N42" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="11:14" x14ac:dyDescent="0.25">
@@ -1387,18 +1387,18 @@
         <v>58</v>
       </c>
       <c r="L43" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M43" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="N43" s="32" t="s">
         <v>81</v>
-      </c>
-      <c r="N43" s="32" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="44" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K44" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L44" s="28"/>
       <c r="M44" s="28"/>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="45" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K45" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L45" s="28"/>
       <c r="M45" s="28"/>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="46" spans="11:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K46" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L46" s="33"/>
       <c r="M46" s="33"/>

</xml_diff>